<commit_message>
Template for Shiny app
</commit_message>
<xml_diff>
--- a/inst/extdata/example_afdata.xlsx
+++ b/inst/extdata/example_afdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewdenwood/Documents/GitHub/tidyepi/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE548F10-71CF-4B44-9A72-787B312319F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5271475-B4CB-2349-805D-2CE12970B955}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{3896AFCD-EDCD-4F42-917C-057C0F965F41}"/>
+    <workbookView xWindow="17880" yWindow="7820" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{3896AFCD-EDCD-4F42-917C-057C0F965F41}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -653,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9725DB6-86CE-4640-B9C8-43A0BE158F01}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,33 +682,25 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43634</v>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0.1</v>
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -721,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE5A38F-6734-594A-BC99-3EAAA734C298}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646F0159-EB9D-DC41-A8D7-60DD6FCECAD9}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,8 +960,9 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="str">
+        <f>"Animal_"&amp;ROW()-1</f>
+        <v>Animal_1</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -994,8 +987,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A11" si="0">"Animal_"&amp;ROW()-1</f>
+        <v>Animal_2</v>
       </c>
       <c r="B3" t="s">
         <v>38</v>
@@ -1020,8 +1014,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>Animal_3</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -1046,8 +1041,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Animal_4</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
@@ -1072,8 +1068,9 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>Animal_5</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -1098,8 +1095,9 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>Animal_6</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
@@ -1124,8 +1122,9 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>Animal_7</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -1150,8 +1149,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>Animal_8</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
@@ -1176,8 +1176,9 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>Animal_9</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -1202,8 +1203,9 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>Animal_10</v>
       </c>
       <c r="B11" t="s">
         <v>56</v>

</xml_diff>